<commit_message>
Directly Uploading everyThing which was left and from here gonna commit regularly
</commit_message>
<xml_diff>
--- a/Java + DSA/DSA question sheet .xlsx
+++ b/Java + DSA/DSA question sheet .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedan\Desktop\WorkSpace\Java+Dsa\Java + DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665209FE-3807-4331-9596-297FD7A2A545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCD008D-6E22-47E2-844A-F489E4BB1268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0A0D14C-2F57-45B0-BFBE-50391B1E0D8C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Questions</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sr no </t>
+  </si>
+  <si>
+    <t>Merge Sort Recurrsion</t>
+  </si>
+  <si>
+    <t>Quick Sort Recurrsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Making Subset of the String given by the User </t>
   </si>
 </sst>
 </file>
@@ -431,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BEA98A-4118-4C20-84E7-A6963AB292FA}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +498,37 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>